<commit_message>
Updated code and result
</commit_message>
<xml_diff>
--- a/modules/cloudsim-examples/src/main/java/org/cloudbus/cloudsim/assignment/Results.xlsx
+++ b/modules/cloudsim-examples/src/main/java/org/cloudbus/cloudsim/assignment/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emon\NSU\DOS\cloudsim-5.0\modules\cloudsim-examples\src\main\java\org\cloudbus\cloudsim\assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE820FD-F56D-42C4-A3D7-4C3B688DC40D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD7AABD-0779-45A6-A601-A43529B33C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
@@ -65,16 +65,16 @@
     <t>Total Host</t>
   </si>
   <si>
-    <t>Comparison of Algorithms (7650 VMs)</t>
+    <t>Comparison of Algorithms (10 VMs vs 10 Host)</t>
   </si>
   <si>
-    <t>Comparison of Algorithms (5000 VMs)</t>
+    <t>Comparison of Algorithms (1000 VMs vs 1000 Hosts)</t>
   </si>
   <si>
-    <t>Comparison of Algorithms (10 VMs)</t>
+    <t>Comparison of Algorithms (5000 VMs vs 5000 Hosts)</t>
   </si>
   <si>
-    <t>Comparison of Algorithms (1000 VMs)</t>
+    <t>Comparison of Algorithms (7650 VMs vs 7650 Hosts)</t>
   </si>
 </sst>
 </file>
@@ -98,18 +98,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -126,6 +120,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,24 +169,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -383,19 +404,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,19 +551,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,16 +698,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
@@ -1114,19 +1135,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>392</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>390</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>392</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>390</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>371</c:v>
+                  <c:v>382</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1273,7 +1294,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>129</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1408,16 +1429,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>608</c:v>
+                  <c:v>601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>610</c:v>
+                  <c:v>601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>608</c:v>
+                  <c:v>601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>610</c:v>
+                  <c:v>601</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>500</c:v>
@@ -1845,19 +1866,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>1994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>1913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1992,10 +2013,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2004,7 +2025,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>587</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2139,19 +2160,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>3002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>3005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2576,19 +2597,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>3068</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>3063</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>3068</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3063</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3939</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2723,19 +2744,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>886</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2870,19 +2891,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4582</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4587</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>4582</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>4587</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>3825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5488,12 +5509,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
@@ -5528,13 +5549,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
@@ -5569,15 +5590,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>42863</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5612,13 +5633,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>48596</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447092</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5911,102 +5932,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="B3" s="7">
         <v>4</v>
       </c>
-      <c r="E3" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3</v>
+      <c r="C3" s="7">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7">
+        <v>4</v>
+      </c>
+      <c r="F3" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
         <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
         <v>5</v>
       </c>
     </row>
@@ -6014,23 +6038,23 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <f>SUM(B3:B5)</f>
         <v>10</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <f>SUM(C3:C5)</f>
         <v>10</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <f>SUM(D3:D5)</f>
         <v>10</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <f>SUM(E3:E5)</f>
         <v>10</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="2">
         <f>SUM(F3:F5)</f>
         <v>10</v>
       </c>
@@ -6049,97 +6073,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11BE434-936A-40B8-BDBF-E06E9EFF137E}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="5"/>
+    <col min="5" max="5" width="15" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
-        <v>392</v>
-      </c>
-      <c r="C3" s="4">
-        <v>390</v>
-      </c>
-      <c r="D3" s="4">
-        <v>392</v>
-      </c>
-      <c r="E3" s="4">
-        <v>390</v>
-      </c>
-      <c r="F3" s="4">
-        <v>371</v>
+      <c r="B3" s="7">
+        <v>399</v>
+      </c>
+      <c r="C3" s="7">
+        <v>399</v>
+      </c>
+      <c r="D3" s="7">
+        <v>399</v>
+      </c>
+      <c r="E3" s="7">
+        <v>399</v>
+      </c>
+      <c r="F3" s="7">
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="8">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="8">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
         <v>0</v>
       </c>
-      <c r="F4" s="4">
-        <v>129</v>
+      <c r="F4" s="8">
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <v>608</v>
-      </c>
-      <c r="C5" s="4">
-        <v>610</v>
-      </c>
-      <c r="D5" s="4">
-        <v>608</v>
-      </c>
-      <c r="E5" s="4">
-        <v>610</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="B5" s="1">
+        <v>601</v>
+      </c>
+      <c r="C5" s="1">
+        <v>601</v>
+      </c>
+      <c r="D5" s="1">
+        <v>601</v>
+      </c>
+      <c r="E5" s="1">
+        <v>601</v>
+      </c>
+      <c r="F5" s="1">
         <v>500</v>
       </c>
     </row>
@@ -6147,23 +6179,23 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <f>SUM(B3:B5)</f>
         <v>1000</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <f>SUM(C3:C5)</f>
         <v>1000</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <f>SUM(D3:D5)</f>
         <v>1000</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <f>SUM(E3:E5)</f>
         <v>1000</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="2">
         <f>SUM(F3:F5)</f>
         <v>1000</v>
       </c>
@@ -6183,122 +6215,130 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3</v>
+      <c r="B3" s="7">
+        <v>1998</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1994</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1998</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1994</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1913</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="B4" s="8">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="C4" s="8">
         <v>1</v>
       </c>
-      <c r="F4" s="4">
-        <v>2</v>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5</v>
+      <c r="B5" s="1">
+        <v>3002</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3005</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3002</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3005</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2500</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <f>SUM(B3:B5)</f>
-        <v>10</v>
-      </c>
-      <c r="C6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="C6" s="2">
         <f>SUM(C3:C5)</f>
-        <v>10</v>
-      </c>
-      <c r="D6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D6" s="2">
         <f>SUM(D3:D5)</f>
-        <v>10</v>
-      </c>
-      <c r="E6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="E6" s="2">
         <f>SUM(E3:E5)</f>
-        <v>10</v>
-      </c>
-      <c r="F6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="F6" s="2">
         <f>SUM(F3:F5)</f>
-        <v>10</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -6314,127 +6354,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5E59E6-8006-40F4-B303-AF45EFCB2B00}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="10.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="5"/>
+    <col min="5" max="5" width="12" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3</v>
+      <c r="B3" s="7">
+        <v>3068</v>
+      </c>
+      <c r="C3" s="7">
+        <v>3063</v>
+      </c>
+      <c r="D3" s="7">
+        <v>3068</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3063</v>
+      </c>
+      <c r="F3" s="7">
+        <v>3939</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="B4" s="8">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2</v>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>886</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>6</v>
-      </c>
-      <c r="E5" s="4">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5</v>
+      <c r="B5" s="1">
+        <v>4582</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4587</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4582</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4587</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3825</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <f>SUM(B3:B5)</f>
-        <v>10</v>
-      </c>
-      <c r="C6" s="5">
+        <v>7650</v>
+      </c>
+      <c r="C6" s="2">
         <f>SUM(C3:C5)</f>
-        <v>10</v>
-      </c>
-      <c r="D6" s="5">
+        <v>7650</v>
+      </c>
+      <c r="D6" s="2">
         <f>SUM(D3:D5)</f>
-        <v>10</v>
-      </c>
-      <c r="E6" s="5">
+        <v>7650</v>
+      </c>
+      <c r="E6" s="2">
         <f>SUM(E3:E5)</f>
-        <v>10</v>
-      </c>
-      <c r="F6" s="5">
+        <v>7650</v>
+      </c>
+      <c r="F6" s="2">
         <f>SUM(F3:F5)</f>
-        <v>10</v>
+        <v>8650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated summary and result excel
</commit_message>
<xml_diff>
--- a/modules/cloudsim-examples/src/main/java/org/cloudbus/cloudsim/assignment/Results.xlsx
+++ b/modules/cloudsim-examples/src/main/java/org/cloudbus/cloudsim/assignment/Results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emon\NSU\DOS\cloudsim-5.0\modules\cloudsim-examples\src\main\java\org\cloudbus\cloudsim\assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD7AABD-0779-45A6-A601-A43529B33C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E643BD3E-AA89-48B5-B531-52A01F15B433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10" sheetId="1" r:id="rId1"/>
-    <sheet name="1000" sheetId="3" r:id="rId2"/>
-    <sheet name="5000" sheetId="4" r:id="rId3"/>
-    <sheet name="7650" sheetId="5" r:id="rId4"/>
+    <sheet name="100" sheetId="6" r:id="rId2"/>
+    <sheet name="1000" sheetId="3" r:id="rId3"/>
+    <sheet name="5000" sheetId="4" r:id="rId4"/>
+    <sheet name="7650" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
   <si>
     <t>BestFit</t>
   </si>
@@ -75,6 +76,9 @@
   </si>
   <si>
     <t>Comparison of Algorithms (7650 VMs vs 7650 Hosts)</t>
+  </si>
+  <si>
+    <t>Comparison of Algorithms (100 VMs vs 100 Host)</t>
   </si>
 </sst>
 </file>
@@ -177,12 +181,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -196,6 +194,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -404,19 +408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -557,13 +561,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -698,16 +702,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
@@ -1016,6 +1020,737 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'100'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Host Over</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'100'!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>BestFit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BestFitDec</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FirstFit</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FirstFitDec</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSVP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100'!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD40-4A04-A016-B717D4A913B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Host Under</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'100'!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>BestFit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BestFitDec</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FirstFit</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FirstFitDec</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSVP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100'!$B$4:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AD40-4A04-A016-B717D4A913B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Host free</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'100'!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>BestFit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BestFitDec</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FirstFit</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FirstFitDec</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CSVP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100'!$B$5:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AD40-4A04-A016-B717D4A913B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="65"/>
+        <c:shape val="box"/>
+        <c:axId val="268500015"/>
+        <c:axId val="394877183"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="268500015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="394877183"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="394877183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="268500015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="60"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="100"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'1000'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1135,19 +1870,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>399</c:v>
+                  <c:v>354</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>399</c:v>
+                  <c:v>353</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>399</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>399</c:v>
+                  <c:v>353</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>382</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1282,19 +2017,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1429,16 +2164,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>601</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>601</c:v>
+                  <c:v>646</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>601</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>601</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>500</c:v>
@@ -1677,7 +2412,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1866,19 +2601,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1998</c:v>
+                  <c:v>1735</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1994</c:v>
+                  <c:v>1734</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1998</c:v>
+                  <c:v>1735</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1994</c:v>
+                  <c:v>1734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1913</c:v>
+                  <c:v>1590</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2019,13 +2754,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>587</c:v>
+                  <c:v>910</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2160,16 +2895,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3002</c:v>
+                  <c:v>3265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3005</c:v>
+                  <c:v>3265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3002</c:v>
+                  <c:v>3264</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3005</c:v>
+                  <c:v>3265</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2500</c:v>
@@ -2408,7 +3143,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2597,19 +3332,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3068</c:v>
+                  <c:v>2659</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3063</c:v>
+                  <c:v>2659</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3068</c:v>
+                  <c:v>2659</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3063</c:v>
+                  <c:v>2659</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3939</c:v>
+                  <c:v>2434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2744,19 +3479,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>886</c:v>
+                  <c:v>1391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2891,16 +3626,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4582</c:v>
+                  <c:v>4990</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4587</c:v>
+                  <c:v>4991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4582</c:v>
+                  <c:v>4990</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4587</c:v>
+                  <c:v>4991</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3825</c:v>
@@ -3287,6 +4022,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="288">
   <cs:axisTitle>
@@ -4950,6 +5722,560 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="288">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="288">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5550,6 +6876,49 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02737C68-B907-465D-8EE1-CF6B994E4406}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5585,7 +6954,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5626,7 +6995,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5932,32 +7301,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5978,40 +7347,40 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5">
         <v>4</v>
       </c>
-      <c r="C3" s="7">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7">
-        <v>4</v>
-      </c>
-      <c r="F3" s="7">
-        <v>5</v>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>1</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
+      <c r="F4" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6019,16 +7388,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1">
         <v>5</v>
@@ -6070,35 +7439,176 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11BE434-936A-40B8-BDBF-E06E9EFF137E}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1B9F12-0D6B-423B-88BC-B2F12830D885}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="15" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5">
+        <v>35</v>
+      </c>
+      <c r="D3" s="5">
+        <v>36</v>
+      </c>
+      <c r="E3" s="5">
+        <v>35</v>
+      </c>
+      <c r="F3" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1">
+        <v>65</v>
+      </c>
+      <c r="D5" s="1">
+        <v>63</v>
+      </c>
+      <c r="E5" s="1">
+        <v>65</v>
+      </c>
+      <c r="F5" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <f>SUM(B3:B5)</f>
+        <v>100</v>
+      </c>
+      <c r="C6" s="2">
+        <f>SUM(C3:C5)</f>
+        <v>100</v>
+      </c>
+      <c r="D6" s="2">
+        <f>SUM(D3:D5)</f>
+        <v>100</v>
+      </c>
+      <c r="E6" s="2">
+        <f>SUM(E3:E5)</f>
+        <v>100</v>
+      </c>
+      <c r="F6" s="2">
+        <f>SUM(F3:F5)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11BE434-936A-40B8-BDBF-E06E9EFF137E}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="15" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6119,40 +7629,40 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
-        <v>399</v>
-      </c>
-      <c r="C3" s="7">
-        <v>399</v>
-      </c>
-      <c r="D3" s="7">
-        <v>399</v>
-      </c>
-      <c r="E3" s="7">
-        <v>399</v>
-      </c>
-      <c r="F3" s="7">
-        <v>382</v>
+      <c r="B3" s="5">
+        <v>354</v>
+      </c>
+      <c r="C3" s="5">
+        <v>353</v>
+      </c>
+      <c r="D3" s="5">
+        <v>355</v>
+      </c>
+      <c r="E3" s="5">
+        <v>353</v>
+      </c>
+      <c r="F3" s="5">
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
         <v>0</v>
       </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
-        <v>118</v>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6160,16 +7670,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>601</v>
+        <v>645</v>
       </c>
       <c r="C5" s="1">
-        <v>601</v>
+        <v>646</v>
       </c>
       <c r="D5" s="1">
-        <v>601</v>
+        <v>645</v>
       </c>
       <c r="E5" s="1">
-        <v>601</v>
+        <v>645</v>
       </c>
       <c r="F5" s="1">
         <v>500</v>
@@ -6193,13 +7703,13 @@
       </c>
       <c r="E6" s="2">
         <f>SUM(E3:E5)</f>
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="F6" s="2">
         <f>SUM(F3:F5)</f>
         <v>1000</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6210,12 +7720,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AC2BE1-86E2-4BB3-8FE2-AC24A49AB73A}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6229,17 +7739,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6260,40 +7770,40 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
-        <v>1998</v>
-      </c>
-      <c r="C3" s="7">
-        <v>1994</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1998</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1994</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1913</v>
+      <c r="B3" s="5">
+        <v>1735</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1734</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1735</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1734</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1590</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>1</v>
       </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="8">
-        <v>587</v>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>910</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6301,16 +7811,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>3002</v>
+        <v>3265</v>
       </c>
       <c r="C5" s="1">
-        <v>3005</v>
+        <v>3265</v>
       </c>
       <c r="D5" s="1">
-        <v>3002</v>
+        <v>3264</v>
       </c>
       <c r="E5" s="1">
-        <v>3005</v>
+        <v>3265</v>
       </c>
       <c r="F5" s="1">
         <v>2500</v>
@@ -6350,36 +7860,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5E59E6-8006-40F4-B303-AF45EFCB2B00}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="10.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="12" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="14.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="10.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="12" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6400,40 +7910,40 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
-        <v>3068</v>
-      </c>
-      <c r="C3" s="7">
-        <v>3063</v>
-      </c>
-      <c r="D3" s="7">
-        <v>3068</v>
-      </c>
-      <c r="E3" s="7">
-        <v>3063</v>
-      </c>
-      <c r="F3" s="7">
-        <v>3939</v>
+      <c r="B3" s="5">
+        <v>2659</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2659</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2659</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2659</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2434</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
         <v>0</v>
       </c>
-      <c r="C4" s="8">
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
         <v>0</v>
       </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
-        <v>886</v>
+      <c r="F4" s="6">
+        <v>1391</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6441,16 +7951,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>4582</v>
+        <v>4990</v>
       </c>
       <c r="C5" s="1">
-        <v>4587</v>
+        <v>4991</v>
       </c>
       <c r="D5" s="1">
-        <v>4582</v>
+        <v>4990</v>
       </c>
       <c r="E5" s="1">
-        <v>4587</v>
+        <v>4991</v>
       </c>
       <c r="F5" s="1">
         <v>3825</v>
@@ -6478,7 +7988,7 @@
       </c>
       <c r="F6" s="2">
         <f>SUM(F3:F5)</f>
-        <v>8650</v>
+        <v>7650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>